<commit_message>
edit to training file
</commit_message>
<xml_diff>
--- a/pipline/examples/output/traning_data.xlsx
+++ b/pipline/examples/output/traning_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WoomBat\source\repos\Woombat84\WNA\pipline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3178C6-E6D3-40A2-87B7-7C9C15608BCC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F43B7FA-3E5F-48AA-8641-51CCD8D2D588}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{AF4D3F67-905C-4ACA-B73D-2EBAF602478B}"/>
   </bookViews>
@@ -415,56 +415,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B25239-478A-406A-BDBF-C57B5BAC8550}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="B1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>